<commit_message>
added sprint 1 backlog, update sprint 0 retro, product backlog
</commit_message>
<xml_diff>
--- a/Milestone 1 Deliverables/Product Backlog.xlsx
+++ b/Milestone 1 Deliverables/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau.sharepoint.com/sites/SEPT-Team/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="259" documentId="D6AE4E6F006198DE85E01EA8692AA13C2D83CCCF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D97C002-34AA-429B-89C1-1CFAD099505E}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="D6AE4E6F006198DE85E01EA8692AA13C2D83CCCF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9B23BED-340B-48A7-B732-B43A0CCE91D8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="lstYears">OFFSET('Product Backlog'!$C$4:$I$4,0,1,1,COUNTA('Product Backlog'!$C$4:$I$4)-1)</definedName>
     <definedName name="SelectedYear">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="59">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -156,9 +156,6 @@
     <t>As a first time visitor, I want to land at a homepage with number of friendly links to useful pages, So that I can navigate the website</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to go to a specific book's page to view more information about it, So that I know about the book being sold</t>
   </si>
   <si>
@@ -214,6 +211,12 @@
   </si>
   <si>
     <t>All Metrics (works up to 25 metrics)</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Sprint1</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -473,25 +476,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -507,11 +498,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -838,7 +835,7 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -912,771 +909,787 @@
       <c r="B5" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="29">
         <v>3</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20" t="s">
+      <c r="G5" s="23"/>
+      <c r="H5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>2</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="30">
         <v>3</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="22"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>3</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="30">
         <v>3</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22" t="s">
+      <c r="G7" s="24"/>
+      <c r="H7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="22"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>4</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22" t="s">
+      <c r="G8" s="24"/>
+      <c r="H8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="22"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="26">
-        <v>3</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22" t="s">
+      <c r="F9" s="30">
+        <v>13</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="22"/>
+      <c r="I9" s="24" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="19">
         <v>6</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="30">
         <v>3</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="24"/>
+      <c r="H10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="22"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="21">
+      <c r="B11" s="20">
         <v>7</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="30">
         <v>5</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22" t="s">
+      <c r="G11" s="24"/>
+      <c r="H11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="22"/>
+      <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>8</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="22" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="30">
         <v>5</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22" t="s">
+      <c r="G12" s="24"/>
+      <c r="H12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="22"/>
+      <c r="I12" s="24"/>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
-      <c r="B13" s="21">
+      <c r="B13" s="20">
         <v>9</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="22" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="30">
         <v>5</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22" t="s">
+      <c r="G13" s="24"/>
+      <c r="H13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="22"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>10</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="22" t="s">
         <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="30">
         <v>3</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22" t="s">
+      <c r="G14" s="24"/>
+      <c r="H14" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="22"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="19">
         <v>11</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="30">
         <v>3</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22" t="s">
+      <c r="G15" s="24"/>
+      <c r="H15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="22"/>
+      <c r="I15" s="24"/>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>12</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="22" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="30">
         <v>5</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22" t="s">
+      <c r="G16" s="24"/>
+      <c r="H16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="22"/>
+      <c r="I16" s="24"/>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <v>13</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="30">
         <v>5</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22" t="s">
+      <c r="G17" s="24"/>
+      <c r="H17" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="22"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
-      <c r="B18" s="21">
+      <c r="B18" s="20">
         <v>14</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="30">
         <v>5</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22" t="s">
+      <c r="G18" s="24"/>
+      <c r="H18" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="22"/>
+      <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
-      <c r="B19" s="21">
+      <c r="B19" s="20">
         <v>15</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="22" t="s">
         <v>28</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="30">
         <v>3</v>
       </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22" t="s">
+      <c r="G19" s="24"/>
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="22"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="19">
         <v>16</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>29</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="30">
         <v>3</v>
       </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22" t="s">
+      <c r="G20" s="24"/>
+      <c r="H20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="22"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
-      <c r="B21" s="21">
+      <c r="B21" s="20">
         <v>17</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="22" t="s">
         <v>30</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="30">
         <v>3</v>
       </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22" t="s">
+      <c r="G21" s="24"/>
+      <c r="H21" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="22"/>
+      <c r="I21" s="24"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
-      <c r="B22" s="21">
+      <c r="B22" s="20">
         <v>18</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="30">
         <v>5</v>
       </c>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22" t="s">
+      <c r="G22" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="22"/>
+      <c r="I22" s="24" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
-      <c r="B23" s="21">
+      <c r="B23" s="20">
         <v>19</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="22" t="s">
         <v>32</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="30">
         <v>3</v>
       </c>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22" t="s">
+      <c r="G23" s="24"/>
+      <c r="H23" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="22"/>
+      <c r="I23" s="24"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
-      <c r="B24" s="21">
+      <c r="B24" s="20">
         <v>20</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="30">
         <v>3</v>
       </c>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22" t="s">
+      <c r="G24" s="24"/>
+      <c r="H24" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="22"/>
+      <c r="I24" s="24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="19">
         <v>21</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="30">
         <v>3</v>
       </c>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22" t="s">
+      <c r="G25" s="24"/>
+      <c r="H25" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="22"/>
+      <c r="I25" s="24"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
-      <c r="B26" s="21">
+      <c r="B26" s="20">
         <v>22</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="22" t="s">
         <v>35</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="30">
         <v>3</v>
       </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22" t="s">
+      <c r="G26" s="24"/>
+      <c r="H26" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="22"/>
+      <c r="I26" s="24"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="19">
         <v>23</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="29">
         <v>3</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20" t="s">
+      <c r="G27" s="23"/>
+      <c r="H27" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="20"/>
+      <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
-      <c r="B28" s="21">
+      <c r="B28" s="20">
         <v>24</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="22" t="s">
         <v>37</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="31">
         <v>20</v>
       </c>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22" t="s">
+      <c r="G28" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="22"/>
+      <c r="I28" s="24" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
-      <c r="B29" s="21">
+      <c r="B29" s="20">
         <v>25</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>39</v>
+      <c r="C29" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22" t="s">
+      <c r="F29" s="31">
+        <v>8</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="22"/>
+      <c r="I29" s="24" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
-      <c r="B30" s="21">
+      <c r="B30" s="20">
         <v>26</v>
       </c>
-      <c r="C30" s="24" t="s">
-        <v>40</v>
+      <c r="C30" s="22" t="s">
+        <v>39</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="E30" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22" t="s">
+      <c r="F30" s="31">
+        <v>5</v>
+      </c>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="22"/>
+      <c r="I30" s="24"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
-      <c r="B31" s="21">
+      <c r="B31" s="20">
         <v>27</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="19">
         <v>28</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
-      <c r="B33" s="21">
+      <c r="B33" s="20">
         <v>29</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
-      <c r="B34" s="21">
+      <c r="B34" s="20">
         <v>30</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
-      <c r="B35" s="21">
+      <c r="B35" s="20">
         <v>31</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="21">
+      <c r="B36" s="20">
         <v>32</v>
       </c>
-      <c r="C36" s="24"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="19">
         <v>33</v>
       </c>
-      <c r="C37" s="24"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
-      <c r="B38" s="21">
+      <c r="B38" s="20">
         <v>34</v>
       </c>
-      <c r="C38" s="24"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
-      <c r="B39" s="21">
+      <c r="B39" s="20">
         <v>35</v>
       </c>
-      <c r="C39" s="24"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
-      <c r="B40" s="21">
+      <c r="B40" s="20">
         <v>36</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
-      <c r="B41" s="21">
+      <c r="B41" s="20">
         <v>37</v>
       </c>
-      <c r="C41" s="24"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="19">
         <v>38</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
-      <c r="B43" s="21">
+      <c r="B43" s="20">
         <v>39</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
-      <c r="B44" s="21">
+      <c r="B44" s="20">
         <v>40</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
-      <c r="B45" s="23"/>
+      <c r="B45" s="21"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
@@ -1687,61 +1700,61 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C47" s="28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C47" s="33" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C48" s="28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C48" s="33" t="s">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="33" t="s">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="33" t="s">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="28" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C51" s="33" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B5:I6 C7:C27 B7:B31 D7:I31 B27:I44">
+  <conditionalFormatting sqref="B5:I6 C7:C27 B7:B31 B27:I44 D7:I31">
     <cfRule type="expression" dxfId="1" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -1770,17 +1783,17 @@
   <sheetData>
     <row r="1" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="e">
         <f>SelectedYear</f>
@@ -1793,7 +1806,7 @@
     </row>
     <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="e">
         <f>C3-1</f>
@@ -1807,7 +1820,7 @@
     <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="e">
         <f ca="1">MATCH(C7,lstYears,0)+1</f>
@@ -1832,7 +1845,7 @@
     </row>
     <row r="7" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="8" t="e">
         <f>D7-1</f>
@@ -2029,7 +2042,7 @@
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2795,8 +2808,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B2353E2A5BD8794FAECD6EBDA6978FDE" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e555e17f0d7e1c0e254458ffcabd1614">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3edec336-ac73-42aa-a558-27fbb502397a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e68329bdc27f61e5d7e3a69169d6d79" ns2:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B2353E2A5BD8794FAECD6EBDA6978FDE" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5f4bc44ba184817ec51d37b52f15f098">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3edec336-ac73-42aa-a558-27fbb502397a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1f960c4d0911bbe4d4de994f384c677b" ns2:_="">
     <xsd:import namespace="3edec336-ac73-42aa-a558-27fbb502397a"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -2808,6 +2827,11 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2838,6 +2862,33 @@
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -2940,12 +2991,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2956,37 +3001,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0900E09A-26E3-4DEF-8D9F-8AD453DFA48C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A35018-99EB-44C4-811D-41831E2986B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3edec336-ac73-42aa-a558-27fbb502397a"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3edec336-ac73-42aa-a558-27fbb502397a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A35018-99EB-44C4-811D-41831E2986B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3edec336-ac73-42aa-a558-27fbb502397a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{053C3F6C-25D2-4689-9715-4694FAE652CD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>